<commit_message>
update response for getting status
- improve scraper performance
</commit_message>
<xml_diff>
--- a/inventory_source_scraper/static/output.xlsx
+++ b/inventory_source_scraper/static/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1470,6 +1470,11 @@
       <c r="D28" t="n">
         <v>1042.72</v>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>987.98</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>No</t>
@@ -1617,6 +1622,11 @@
       <c r="D32" t="n">
         <v>878.3099999999999</v>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>987.98</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>No</t>
@@ -7851,7 +7861,6 @@
       <c r="D220" t="n">
         <v>153.09</v>
       </c>
-      <c r="E220" t="inlineStr"/>
       <c r="F220" t="inlineStr">
         <is>
           <t>No</t>
@@ -7863,6 +7872,4795 @@
       </c>
       <c r="H220">
         <f>E220-D220</f>
+        <v/>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G221">
+        <f>(E221-D221)/D221*100</f>
+        <v/>
+      </c>
+      <c r="H221">
+        <f>E221-D221</f>
+        <v/>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G222">
+        <f>(E222-D222)/D222*100</f>
+        <v/>
+      </c>
+      <c r="H222">
+        <f>E222-D222</f>
+        <v/>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Crick Ksa2225    Pink Laminated Blued</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G223">
+        <f>(E223-D223)/D223*100</f>
+        <v/>
+      </c>
+      <c r="H223">
+        <f>E223-D223</f>
+        <v/>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2225    Pink Laminated Blued</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G224">
+        <f>(E224-D224)/D224*100</f>
+        <v/>
+      </c>
+      <c r="H224">
+        <f>E224-D224</f>
+        <v/>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KSA PINK LAMINATED 22LR </t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>156</v>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G225">
+        <f>(E225-D225)/D225*100</f>
+        <v/>
+      </c>
+      <c r="H225">
+        <f>E225-D225</f>
+        <v/>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G226">
+        <f>(E226-D226)/D226*100</f>
+        <v/>
+      </c>
+      <c r="H226">
+        <f>E226-D226</f>
+        <v/>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G227">
+        <f>(E227-D227)/D227*100</f>
+        <v/>
+      </c>
+      <c r="H227">
+        <f>E227-D227</f>
+        <v/>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - Blued/pink Laminate</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>162.4</v>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G228">
+        <f>(E228-D228)/D228*100</f>
+        <v/>
+      </c>
+      <c r="H228">
+        <f>E228-D228</f>
+        <v/>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/pink Lam</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>611613022251</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Bill Hicks Co.</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>156</v>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G229">
+        <f>(E229-D229)/D229*100</f>
+        <v/>
+      </c>
+      <c r="H229">
+        <f>E229-D229</f>
+        <v/>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>KSA 22LR SS/PNK LAM</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>165.95</v>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G230">
+        <f>(E230-D230)/D230*100</f>
+        <v/>
+      </c>
+      <c r="H230">
+        <f>E230-D230</f>
+        <v/>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/pink Lam</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>169.08</v>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G231">
+        <f>(E231-D231)/D231*100</f>
+        <v/>
+      </c>
+      <c r="H231">
+        <f>E231-D231</f>
+        <v/>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Pink 22s/l/lr 16.125"</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>170</v>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G232">
+        <f>(E232-D232)/D232*100</f>
+        <v/>
+      </c>
+      <c r="H232">
+        <f>E232-D232</f>
+        <v/>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>172.88</v>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G233">
+        <f>(E233-D233)/D233*100</f>
+        <v/>
+      </c>
+      <c r="H233">
+        <f>E233-D233</f>
+        <v/>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>172.88</v>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G234">
+        <f>(E234-D234)/D234*100</f>
+        <v/>
+      </c>
+      <c r="H234">
+        <f>E234-D234</f>
+        <v/>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Crickett 22lr Pink Lam Ss Brl</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>172.25</v>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G235">
+        <f>(E235-D235)/D235*100</f>
+        <v/>
+      </c>
+      <c r="H235">
+        <f>E235-D235</f>
+        <v/>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>KSA 226 22LR YT 16.1 SS PNK 1</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>DAVEY CRICKETT</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>170.97</v>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G236">
+        <f>(E236-D236)/D236*100</f>
+        <v/>
+      </c>
+      <c r="H236">
+        <f>E236-D236</f>
+        <v/>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>165.51</v>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G237">
+        <f>(E237-D237)/D237*100</f>
+        <v/>
+      </c>
+      <c r="H237">
+        <f>E237-D237</f>
+        <v/>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>165.51</v>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G238">
+        <f>(E238-D238)/D238*100</f>
+        <v/>
+      </c>
+      <c r="H238">
+        <f>E238-D238</f>
+        <v/>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Crick Ksa2226    Pink Laminated S/s</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>169.67</v>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G239">
+        <f>(E239-D239)/D239*100</f>
+        <v/>
+      </c>
+      <c r="H239">
+        <f>E239-D239</f>
+        <v/>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2226    Pink Laminated S/s</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>169.67</v>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G240">
+        <f>(E240-D240)/D240*100</f>
+        <v/>
+      </c>
+      <c r="H240">
+        <f>E240-D240</f>
+        <v/>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - S/s Pink Laminate</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>175.84</v>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G241">
+        <f>(E241-D241)/D241*100</f>
+        <v/>
+      </c>
+      <c r="H241">
+        <f>E241-D241</f>
+        <v/>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>165.51</v>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G242">
+        <f>(E242-D242)/D242*100</f>
+        <v/>
+      </c>
+      <c r="H242">
+        <f>E242-D242</f>
+        <v/>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pink Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>165.51</v>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G243">
+        <f>(E243-D243)/D243*100</f>
+        <v/>
+      </c>
+      <c r="H243">
+        <f>E243-D243</f>
+        <v/>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/pink Lam</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>611613022268</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Lipseys</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>169.08</v>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G244">
+        <f>(E244-D244)/D244*100</f>
+        <v/>
+      </c>
+      <c r="H244">
+        <f>E244-D244</f>
+        <v/>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>KSA 22LR BLU/PUR LAM</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>152.95</v>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G245">
+        <f>(E245-D245)/D245*100</f>
+        <v/>
+      </c>
+      <c r="H245">
+        <f>E245-D245</f>
+        <v/>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/purple Lam</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>157.89</v>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G246">
+        <f>(E246-D246)/D246*100</f>
+        <v/>
+      </c>
+      <c r="H246">
+        <f>E246-D246</f>
+        <v/>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Purple 22s/l/lr</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>161.11</v>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G247">
+        <f>(E247-D247)/D247*100</f>
+        <v/>
+      </c>
+      <c r="H247">
+        <f>E247-D247</f>
+        <v/>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Ksa Crickett 22lr Rfl Purp Lam</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>162.99</v>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G248">
+        <f>(E248-D248)/D248*100</f>
+        <v/>
+      </c>
+      <c r="H248">
+        <f>E248-D248</f>
+        <v/>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>159.66</v>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G249">
+        <f>(E249-D249)/D249*100</f>
+        <v/>
+      </c>
+      <c r="H249">
+        <f>E249-D249</f>
+        <v/>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>159.66</v>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G250">
+        <f>(E250-D250)/D250*100</f>
+        <v/>
+      </c>
+      <c r="H250">
+        <f>E250-D250</f>
+        <v/>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Crickett 22lr Purple Lam Bl Brl</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>155</v>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G251">
+        <f>(E251-D251)/D251*100</f>
+        <v/>
+      </c>
+      <c r="H251">
+        <f>E251-D251</f>
+        <v/>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>KSA 227 22LR YTH 16.1 BL PRP 1</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>DAVEY CRICKETT</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>153.09</v>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G252">
+        <f>(E252-D252)/D252*100</f>
+        <v/>
+      </c>
+      <c r="H252">
+        <f>E252-D252</f>
+        <v/>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G253">
+        <f>(E253-D253)/D253*100</f>
+        <v/>
+      </c>
+      <c r="H253">
+        <f>E253-D253</f>
+        <v/>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G254">
+        <f>(E254-D254)/D254*100</f>
+        <v/>
+      </c>
+      <c r="H254">
+        <f>E254-D254</f>
+        <v/>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Crick Ksa2227    Purple Laminated Blue</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G255">
+        <f>(E255-D255)/D255*100</f>
+        <v/>
+      </c>
+      <c r="H255">
+        <f>E255-D255</f>
+        <v/>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2227    Purple Laminated Blue</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G256">
+        <f>(E256-D256)/D256*100</f>
+        <v/>
+      </c>
+      <c r="H256">
+        <f>E256-D256</f>
+        <v/>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KSA PURPLE LAMINATED 22L </t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>151.32</v>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G257">
+        <f>(E257-D257)/D257*100</f>
+        <v/>
+      </c>
+      <c r="H257">
+        <f>E257-D257</f>
+        <v/>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G258">
+        <f>(E258-D258)/D258*100</f>
+        <v/>
+      </c>
+      <c r="H258">
+        <f>E258-D258</f>
+        <v/>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - Blued/purple Laminate</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>162.4</v>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G259">
+        <f>(E259-D259)/D259*100</f>
+        <v/>
+      </c>
+      <c r="H259">
+        <f>E259-D259</f>
+        <v/>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>152.44</v>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G260">
+        <f>(E260-D260)/D260*100</f>
+        <v/>
+      </c>
+      <c r="H260">
+        <f>E260-D260</f>
+        <v/>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/purple Lam</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>611613022275</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Bill Hicks Co.</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>151.32</v>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G261">
+        <f>(E261-D261)/D261*100</f>
+        <v/>
+      </c>
+      <c r="H261">
+        <f>E261-D261</f>
+        <v/>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>KSA 22LR SS/PUR LAM</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>165.95</v>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G262">
+        <f>(E262-D262)/D262*100</f>
+        <v/>
+      </c>
+      <c r="H262">
+        <f>E262-D262</f>
+        <v/>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/purple Lam</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>169.08</v>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G263">
+        <f>(E263-D263)/D263*100</f>
+        <v/>
+      </c>
+      <c r="H263">
+        <f>E263-D263</f>
+        <v/>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Purple 22s/l/lr</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>174.44</v>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G264">
+        <f>(E264-D264)/D264*100</f>
+        <v/>
+      </c>
+      <c r="H264">
+        <f>E264-D264</f>
+        <v/>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Pur Lam St Bbl</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>149.99</v>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G265">
+        <f>(E265-D265)/D265*100</f>
+        <v/>
+      </c>
+      <c r="H265">
+        <f>E265-D265</f>
+        <v/>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Crick Ksa2228    Purple Laminated S/s</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>169.67</v>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G266">
+        <f>(E266-D266)/D266*100</f>
+        <v/>
+      </c>
+      <c r="H266">
+        <f>E266-D266</f>
+        <v/>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2228    Purple Laminated S/s</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>169.67</v>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G267">
+        <f>(E267-D267)/D267*100</f>
+        <v/>
+      </c>
+      <c r="H267">
+        <f>E267-D267</f>
+        <v/>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/purple Lam</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Lipseys</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>169.08</v>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G268">
+        <f>(E268-D268)/D268*100</f>
+        <v/>
+      </c>
+      <c r="H268">
+        <f>E268-D268</f>
+        <v/>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - S/s Purple Laminate</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>611613022282</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>175.84</v>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G269">
+        <f>(E269-D269)/D269*100</f>
+        <v/>
+      </c>
+      <c r="H269">
+        <f>E269-D269</f>
+        <v/>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>KSA 22LR BLU/ORG&amp;BLK LAM</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>611613022312</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>152.95</v>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G270">
+        <f>(E270-D270)/D270*100</f>
+        <v/>
+      </c>
+      <c r="H270">
+        <f>E270-D270</f>
+        <v/>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/blk-ornge Lam</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>611613022312</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>157.89</v>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G271">
+        <f>(E271-D271)/D271*100</f>
+        <v/>
+      </c>
+      <c r="H271">
+        <f>E271-D271</f>
+        <v/>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Blk/org 22s/l/lr</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>611613022312</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>161.11</v>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G272">
+        <f>(E272-D272)/D272*100</f>
+        <v/>
+      </c>
+      <c r="H272">
+        <f>E272-D272</f>
+        <v/>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/blk-ornge Lam</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>611613022312</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Lipseys</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>157.89</v>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G273">
+        <f>(E273-D273)/D273*100</f>
+        <v/>
+      </c>
+      <c r="H273">
+        <f>E273-D273</f>
+        <v/>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>KSA 22LR SS/ORG&amp;BLK LAM</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>611613022329</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>165.95</v>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G274">
+        <f>(E274-D274)/D274*100</f>
+        <v/>
+      </c>
+      <c r="H274">
+        <f>E274-D274</f>
+        <v/>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/blk-ornge Lam</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>611613022329</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>169.08</v>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G275">
+        <f>(E275-D275)/D275*100</f>
+        <v/>
+      </c>
+      <c r="H275">
+        <f>E275-D275</f>
+        <v/>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/blk-ornge Lam</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>611613022329</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Lipseys</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>169.08</v>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G276">
+        <f>(E276-D276)/D276*100</f>
+        <v/>
+      </c>
+      <c r="H276">
+        <f>E276-D276</f>
+        <v/>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>KSA 22LR MY 1ST RF SS/TAN SYN</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>123.95</v>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G277">
+        <f>(E277-D277)/D277*100</f>
+        <v/>
+      </c>
+      <c r="H277">
+        <f>E277-D277</f>
+        <v/>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Dtan First Rfl</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>131.11</v>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G278">
+        <f>(E278-D278)/D278*100</f>
+        <v/>
+      </c>
+      <c r="H278">
+        <f>E278-D278</f>
+        <v/>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Tan Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>119.99</v>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G279">
+        <f>(E279-D279)/D279*100</f>
+        <v/>
+      </c>
+      <c r="H279">
+        <f>E279-D279</f>
+        <v/>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/tan</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>126.31</v>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G280">
+        <f>(E280-D280)/D280*100</f>
+        <v/>
+      </c>
+      <c r="H280">
+        <f>E280-D280</f>
+        <v/>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Crick Ksa2243    Desert Tan S/s  (mfr)</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G281">
+        <f>(E281-D281)/D281*100</f>
+        <v/>
+      </c>
+      <c r="H281">
+        <f>E281-D281</f>
+        <v/>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2243    Desert Tan S/s  (mfr)</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G282">
+        <f>(E282-D282)/D282*100</f>
+        <v/>
+      </c>
+      <c r="H282">
+        <f>E282-D282</f>
+        <v/>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - S/s Desert Tan</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G283">
+        <f>(E283-D283)/D283*100</f>
+        <v/>
+      </c>
+      <c r="H283">
+        <f>E283-D283</f>
+        <v/>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/tan</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>611613022435</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Lipseys</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>126.31</v>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G284">
+        <f>(E284-D284)/D284*100</f>
+        <v/>
+      </c>
+      <c r="H284">
+        <f>E284-D284</f>
+        <v/>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>KSA 22LR BLU/BLK LAM</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>152.95</v>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G285">
+        <f>(E285-D285)/D285*100</f>
+        <v/>
+      </c>
+      <c r="H285">
+        <f>E285-D285</f>
+        <v/>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/black Lam</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>157.89</v>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G286">
+        <f>(E286-D286)/D286*100</f>
+        <v/>
+      </c>
+      <c r="H286">
+        <f>E286-D286</f>
+        <v/>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Blk 22s/l/lr 16.125"</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>161.11</v>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G287">
+        <f>(E287-D287)/D287*100</f>
+        <v/>
+      </c>
+      <c r="H287">
+        <f>E287-D287</f>
+        <v/>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>159.66</v>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G288">
+        <f>(E288-D288)/D288*100</f>
+        <v/>
+      </c>
+      <c r="H288">
+        <f>E288-D288</f>
+        <v/>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Crickett 22lr Blk Lam</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>152.5</v>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G289">
+        <f>(E289-D289)/D289*100</f>
+        <v/>
+      </c>
+      <c r="H289">
+        <f>E289-D289</f>
+        <v/>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>159.66</v>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G290">
+        <f>(E290-D290)/D290*100</f>
+        <v/>
+      </c>
+      <c r="H290">
+        <f>E290-D290</f>
+        <v/>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>159.66</v>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G291">
+        <f>(E291-D291)/D291*100</f>
+        <v/>
+      </c>
+      <c r="H291">
+        <f>E291-D291</f>
+        <v/>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>159.66</v>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G292">
+        <f>(E292-D292)/D292*100</f>
+        <v/>
+      </c>
+      <c r="H292">
+        <f>E292-D292</f>
+        <v/>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Crick Ksa2244    Black Laminated</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G293">
+        <f>(E293-D293)/D293*100</f>
+        <v/>
+      </c>
+      <c r="H293">
+        <f>E293-D293</f>
+        <v/>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2244    Black Laminated</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G294">
+        <f>(E294-D294)/D294*100</f>
+        <v/>
+      </c>
+      <c r="H294">
+        <f>E294-D294</f>
+        <v/>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - Blued/black Laminate</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>162.4</v>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G295">
+        <f>(E295-D295)/D295*100</f>
+        <v/>
+      </c>
+      <c r="H295">
+        <f>E295-D295</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/black Lam</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>611613022442</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Sports South</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>157.16</v>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G296">
+        <f>(E296-D296)/D296*100</f>
+        <v/>
+      </c>
+      <c r="H296">
+        <f>E296-D296</f>
+        <v/>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>KSA 22LR MY 1ST RF SS/BLK SYN</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>123.95</v>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G297">
+        <f>(E297-D297)/D297*100</f>
+        <v/>
+      </c>
+      <c r="H297">
+        <f>E297-D297</f>
+        <v/>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/black Syn</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>128.49</v>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G298">
+        <f>(E298-D298)/D298*100</f>
+        <v/>
+      </c>
+      <c r="H298">
+        <f>E298-D298</f>
+        <v/>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Blk First Rfl</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>131.11</v>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G299">
+        <f>(E299-D299)/D299*100</f>
+        <v/>
+      </c>
+      <c r="H299">
+        <f>E299-D299</f>
+        <v/>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>129.93</v>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G300">
+        <f>(E300-D300)/D300*100</f>
+        <v/>
+      </c>
+      <c r="H300">
+        <f>E300-D300</f>
+        <v/>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>129.93</v>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G301">
+        <f>(E301-D301)/D301*100</f>
+        <v/>
+      </c>
+      <c r="H301">
+        <f>E301-D301</f>
+        <v/>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Crickett 22lr Blk Syn Ss Brl</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>130</v>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G302">
+        <f>(E302-D302)/D302*100</f>
+        <v/>
+      </c>
+      <c r="H302">
+        <f>E302-D302</f>
+        <v/>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>123.04</v>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G303">
+        <f>(E303-D303)/D303*100</f>
+        <v/>
+      </c>
+      <c r="H303">
+        <f>E303-D303</f>
+        <v/>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>123.04</v>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G304">
+        <f>(E304-D304)/D304*100</f>
+        <v/>
+      </c>
+      <c r="H304">
+        <f>E304-D304</f>
+        <v/>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Crick Ksa2245    Blk Syn S/s     (mfr)</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G305">
+        <f>(E305-D305)/D305*100</f>
+        <v/>
+      </c>
+      <c r="H305">
+        <f>E305-D305</f>
+        <v/>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2245    Blk Syn S/s     (mfr)</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G306">
+        <f>(E306-D306)/D306*100</f>
+        <v/>
+      </c>
+      <c r="H306">
+        <f>E306-D306</f>
+        <v/>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22lr - S/s Black Synthetic</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>132.45</v>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G307">
+        <f>(E307-D307)/D307*100</f>
+        <v/>
+      </c>
+      <c r="H307">
+        <f>E307-D307</f>
+        <v/>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>123.04</v>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G308">
+        <f>(E308-D308)/D308*100</f>
+        <v/>
+      </c>
+      <c r="H308">
+        <f>E308-D308</f>
+        <v/>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Blk Syn St Bbl</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>123.04</v>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G309">
+        <f>(E309-D309)/D309*100</f>
+        <v/>
+      </c>
+      <c r="H309">
+        <f>E309-D309</f>
+        <v/>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>KSA BLK SYN 22LR MY FIRST RIFLE SS</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>126</v>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G310">
+        <f>(E310-D310)/D310*100</f>
+        <v/>
+      </c>
+      <c r="H310">
+        <f>E310-D310</f>
+        <v/>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Ss/black Syn</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>611613022459</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Bill Hicks Co.</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>126</v>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G311">
+        <f>(E311-D311)/D311*100</f>
+        <v/>
+      </c>
+      <c r="H311">
+        <f>E311-D311</f>
+        <v/>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>KSA 22LR BLU/R&amp;W&amp;B LAM</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>152.95</v>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G312">
+        <f>(E312-D312)/D312*100</f>
+        <v/>
+      </c>
+      <c r="H312">
+        <f>E312-D312</f>
+        <v/>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/rd-wht-bl Lam</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>157.89</v>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G313">
+        <f>(E313-D313)/D313*100</f>
+        <v/>
+      </c>
+      <c r="H313">
+        <f>E313-D313</f>
+        <v/>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Red/wht/blu 22s/l/lr</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>161.11</v>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G314">
+        <f>(E314-D314)/D314*100</f>
+        <v/>
+      </c>
+      <c r="H314">
+        <f>E314-D314</f>
+        <v/>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Crickett 22lr R/w/b Lam Bl Brl</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>155</v>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G315">
+        <f>(E315-D315)/D315*100</f>
+        <v/>
+      </c>
+      <c r="H315">
+        <f>E315-D315</f>
+        <v/>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>KSA 253 22LR 16.1 BL R/W/B 1</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>DAVEY CRICKETT</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>153.09</v>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G316">
+        <f>(E316-D316)/D316*100</f>
+        <v/>
+      </c>
+      <c r="H316">
+        <f>E316-D316</f>
+        <v/>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr Rw&amp;b Lam Bl Bbl</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>139.99</v>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G317">
+        <f>(E317-D317)/D317*100</f>
+        <v/>
+      </c>
+      <c r="H317">
+        <f>E317-D317</f>
+        <v/>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>CRICK KSA2253    RED/WHITE/BLUE</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>131.32</v>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G318">
+        <f>(E318-D318)/D318*100</f>
+        <v/>
+      </c>
+      <c r="H318">
+        <f>E318-D318</f>
+        <v/>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr Bl/rd-wht-bl Lam</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>611613022534</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Lipseys</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>157.89</v>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G319">
+        <f>(E319-D319)/D319*100</f>
+        <v/>
+      </c>
+      <c r="H319">
+        <f>E319-D319</f>
+        <v/>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>KSA 22WMR BLU/MOBU</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>151.95</v>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G320">
+        <f>(E320-D320)/D320*100</f>
+        <v/>
+      </c>
+      <c r="H320">
+        <f>E320-D320</f>
+        <v/>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22mag Bl/breakup Camo</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>156.8</v>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G321">
+        <f>(E321-D321)/D321*100</f>
+        <v/>
+      </c>
+      <c r="H321">
+        <f>E321-D321</f>
+        <v/>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt Mobu 22wmr 16.125"</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>160</v>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G322">
+        <f>(E322-D322)/D322*100</f>
+        <v/>
+      </c>
+      <c r="H322">
+        <f>E322-D322</f>
+        <v/>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Crickett 22mag Mobu Blued</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>155.25</v>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G323">
+        <f>(E323-D323)/D323*100</f>
+        <v/>
+      </c>
+      <c r="H323">
+        <f>E323-D323</f>
+        <v/>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Crick Ksa2284    M-oak Break-up Blue  22mag</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>158.19</v>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G324">
+        <f>(E324-D324)/D324*100</f>
+        <v/>
+      </c>
+      <c r="H324">
+        <f>E324-D324</f>
+        <v/>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2284    M-oak Break-up Blue  22mag</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>158.19</v>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G325">
+        <f>(E325-D325)/D325*100</f>
+        <v/>
+      </c>
+      <c r="H325">
+        <f>E325-D325</f>
+        <v/>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>KSA MOSSY OAK COUNTRY BLUED 22MAG</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>154</v>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G326">
+        <f>(E326-D326)/D326*100</f>
+        <v/>
+      </c>
+      <c r="H326">
+        <f>E326-D326</f>
+        <v/>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22mag Bl/breakup Camo</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>611613022848</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Bill Hicks Co.</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>154</v>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G327">
+        <f>(E327-D327)/D327*100</f>
+        <v/>
+      </c>
+      <c r="H327">
+        <f>E327-D327</f>
+        <v/>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>KSA 22WMR SS/MOBU</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>611613022947</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>164.95</v>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G328">
+        <f>(E328-D328)/D328*100</f>
+        <v/>
+      </c>
+      <c r="H328">
+        <f>E328-D328</f>
+        <v/>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Crick Ksa2294    M-oak Break-up S/s   22mag</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>611613022947</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>169.12</v>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G329">
+        <f>(E329-D329)/D329*100</f>
+        <v/>
+      </c>
+      <c r="H329">
+        <f>E329-D329</f>
+        <v/>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2294    M-oak Break-up S/s   22mag</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>611613022947</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>169.12</v>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G330">
+        <f>(E330-D330)/D330*100</f>
+        <v/>
+      </c>
+      <c r="H330">
+        <f>E330-D330</f>
+        <v/>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Crick Ksa2294    M-oak Break-up S/s   22mag</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>611613022947</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>Sports South</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>169.12</v>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G331">
+        <f>(E331-D331)/D331*100</f>
+        <v/>
+      </c>
+      <c r="H331">
+        <f>E331-D331</f>
+        <v/>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>KSA 22WMR SS/BLK SYN</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>611613022954</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>128.95</v>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G332">
+        <f>(E332-D332)/D332*100</f>
+        <v/>
+      </c>
+      <c r="H332">
+        <f>E332-D332</f>
+        <v/>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Crick Ksa2295    Black Syn S/s        22mag</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>611613022954</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>134.29</v>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G333">
+        <f>(E333-D333)/D333*100</f>
+        <v/>
+      </c>
+      <c r="H333">
+        <f>E333-D333</f>
+        <v/>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2295    Black Syn S/s        22mag</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>611613022954</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>134.29</v>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G334">
+        <f>(E334-D334)/D334*100</f>
+        <v/>
+      </c>
+      <c r="H334">
+        <f>E334-D334</f>
+        <v/>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Crick Ksa2295    Black Syn S/s        22mag</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>611613022954</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Sports South</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>134.29</v>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G335">
+        <f>(E335-D335)/D335*100</f>
+        <v/>
+      </c>
+      <c r="H335">
+        <f>E335-D335</f>
+        <v/>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>KSA 22LR ADULT BLU/PNK LAM</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>611613022985</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>170.95</v>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G336">
+        <f>(E336-D336)/D336*100</f>
+        <v/>
+      </c>
+      <c r="H336">
+        <f>E336-D336</f>
+        <v/>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>KSA 22LR ADULT BLU/WLNT</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>611613023005</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>149.99</v>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G337">
+        <f>(E337-D337)/D337*100</f>
+        <v/>
+      </c>
+      <c r="H337">
+        <f>E337-D337</f>
+        <v/>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>CRICK KSA2300    ADULT WALNUT  BLUE</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>611613023005</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>141.12</v>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G338">
+        <f>(E338-D338)/D338*100</f>
+        <v/>
+      </c>
+      <c r="H338">
+        <f>E338-D338</f>
+        <v/>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>KSA 22WMR BLU/WLNT</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>611613023388</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>147.95</v>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G339">
+        <f>(E339-D339)/D339*100</f>
+        <v/>
+      </c>
+      <c r="H339">
+        <f>E339-D339</f>
+        <v/>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Crick Ksa2338    Walnut Blue</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>611613023388</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>153.64</v>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G340">
+        <f>(E340-D340)/D340*100</f>
+        <v/>
+      </c>
+      <c r="H340">
+        <f>E340-D340</f>
+        <v/>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa2338    Walnut Blue</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>611613023388</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>153.64</v>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G341">
+        <f>(E341-D341)/D341*100</f>
+        <v/>
+      </c>
+      <c r="H341">
+        <f>E341-D341</f>
+        <v/>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KSA WALNUT BLUED 22MAG </t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>611613023388</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>150</v>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G342">
+        <f>(E342-D342)/D342*100</f>
+        <v/>
+      </c>
+      <c r="H342">
+        <f>E342-D342</f>
+        <v/>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22wmr - Blued/walnut</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>611613023388</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>156.8</v>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G343">
+        <f>(E343-D343)/D343*100</f>
+        <v/>
+      </c>
+      <c r="H343">
+        <f>E343-D343</f>
+        <v/>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>Crickett Rifle G2 .22wmr - Blued/walnut</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>611613023388</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Bill Hicks Co.</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>150</v>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G344">
+        <f>(E344-D344)/D344*100</f>
+        <v/>
+      </c>
+      <c r="H344">
+        <f>E344-D344</f>
+        <v/>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>KSA 22LR TARGET TH BLU/PUR</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>611613025276</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>178.95</v>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G345">
+        <f>(E345-D345)/D345*100</f>
+        <v/>
+      </c>
+      <c r="H345">
+        <f>E345-D345</f>
+        <v/>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>KSA 22LR TARGET TH BLU/WLNT</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>611613025382</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>178.95</v>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G346">
+        <f>(E346-D346)/D346*100</f>
+        <v/>
+      </c>
+      <c r="H346">
+        <f>E346-D346</f>
+        <v/>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>Ksa Target Model 22lr Walnut</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>611613025382</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>185</v>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G347">
+        <f>(E347-D347)/D347*100</f>
+        <v/>
+      </c>
+      <c r="H347">
+        <f>E347-D347</f>
+        <v/>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>KSA 22LR TARGET TH BLU/BLK</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>611613025443</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>178.95</v>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G348">
+        <f>(E348-D348)/D348*100</f>
+        <v/>
+      </c>
+      <c r="H348">
+        <f>E348-D348</f>
+        <v/>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>Crick Ksa2544    Black Tgt Model</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>611613025443</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>182.24</v>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G349">
+        <f>(E349-D349)/D349*100</f>
+        <v/>
+      </c>
+      <c r="H349">
+        <f>E349-D349</f>
+        <v/>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>Crickett Black Target, Crick Ksa2544    Black Tgt Model</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>611613025443</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>182.24</v>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G350">
+        <f>(E350-D350)/D350*100</f>
+        <v/>
+      </c>
+      <c r="H350">
+        <f>E350-D350</f>
+        <v/>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>Crick Ksa2544    Black Tgt Model</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>611613025443</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Sports South</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>182.24</v>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G351">
+        <f>(E351-D351)/D351*100</f>
+        <v/>
+      </c>
+      <c r="H351">
+        <f>E351-D351</f>
+        <v/>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>KSA 22LR TARGET TH BLU/BWN</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>611613025559</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>178.95</v>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G352">
+        <f>(E352-D352)/D352*100</f>
+        <v/>
+      </c>
+      <c r="H352">
+        <f>E352-D352</f>
+        <v/>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>Crickett 22lr Ext Th Brown Target M</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>611613025559</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>CRICKETT, KEYSTONE</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>195</v>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G353">
+        <f>(E353-D353)/D353*100</f>
+        <v/>
+      </c>
+      <c r="H353">
+        <f>E353-D353</f>
+        <v/>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>KSA 22LR TARGET TH SS/WLNT</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>611613026389</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>191.95</v>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G354">
+        <f>(E354-D354)/D354*100</f>
+        <v/>
+      </c>
+      <c r="H354">
+        <f>E354-D354</f>
+        <v/>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>KSA 22LR SS/ONE NATION</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>159.95</v>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G355">
+        <f>(E355-D355)/D355*100</f>
+        <v/>
+      </c>
+      <c r="H355">
+        <f>E355-D355</f>
+        <v/>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr 1 Nation St Bbl</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>166.27</v>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G356">
+        <f>(E356-D356)/D356*100</f>
+        <v/>
+      </c>
+      <c r="H356">
+        <f>E356-D356</f>
+        <v/>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr One Nation Ss</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>164.42</v>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G357">
+        <f>(E357-D357)/D357*100</f>
+        <v/>
+      </c>
+      <c r="H357">
+        <f>E357-D357</f>
+        <v/>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Ksa  Crkt One Nation 22lr</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>KSA - KEYSTONE SPORTING ARMS</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>167.77</v>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G358">
+        <f>(E358-D358)/D358*100</f>
+        <v/>
+      </c>
+      <c r="H358">
+        <f>E358-D358</f>
+        <v/>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr 1 Nation St Bbl</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>166.27</v>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G359">
+        <f>(E359-D359)/D359*100</f>
+        <v/>
+      </c>
+      <c r="H359">
+        <f>E359-D359</f>
+        <v/>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr 1 Nation St Bbl</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>166.27</v>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G360">
+        <f>(E360-D360)/D360*100</f>
+        <v/>
+      </c>
+      <c r="H360">
+        <f>E360-D360</f>
+        <v/>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>KSA 169 22LR 16.1 SS 1NATN 1</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>DAVEY CRICKETT</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>165.38</v>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G361">
+        <f>(E361-D361)/D361*100</f>
+        <v/>
+      </c>
+      <c r="H361">
+        <f>E361-D361</f>
+        <v/>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>Ksa Crickett G2 22lr 1 Nation St Bbl</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>166.27</v>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G362">
+        <f>(E362-D362)/D362*100</f>
+        <v/>
+      </c>
+      <c r="H362">
+        <f>E362-D362</f>
+        <v/>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Crick Ksa3169    One Nation S/s</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>162.97</v>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G363">
+        <f>(E363-D363)/D363*100</f>
+        <v/>
+      </c>
+      <c r="H363">
+        <f>E363-D363</f>
+        <v/>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Crickett Crickett, Crick Ksa3169    One Nation S/s</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>Crickett</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>162.97</v>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G364">
+        <f>(E364-D364)/D364*100</f>
+        <v/>
+      </c>
+      <c r="H364">
+        <f>E364-D364</f>
+        <v/>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Keystone Sporting Arms Crickett 22lr One Nation Ss</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>Bill Hicks Co.</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>162</v>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G365">
+        <f>(E365-D365)/D365*100</f>
+        <v/>
+      </c>
+      <c r="H365">
+        <f>E365-D365</f>
+        <v/>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>CRICKET ONE NATION SERIE 22LR SS</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>611613031697</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>KEYSTONE SPORTING ARMS, LLC</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>162</v>
+      </c>
+      <c r="E366" t="inlineStr"/>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G366">
+        <f>(E366-D366)/D366*100</f>
+        <v/>
+      </c>
+      <c r="H366">
+        <f>E366-D366</f>
         <v/>
       </c>
     </row>

</xml_diff>